<commit_message>
added adaptibility to all pages
</commit_message>
<xml_diff>
--- a/vendor/Ассортимент_песен.xlsx
+++ b/vendor/Ассортимент_песен.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Учебные задания\УИРС_Победа\vendor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Учебные задания\УИРС_5_семестр\УИРС_Победа\vendor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AFDFF3E-D01F-464E-AA85-8CA1B328F8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8622D338-616E-4836-8091-E2C02DCAF769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{40F30BFA-022F-4FBF-8F9A-518757B745B0}"/>
   </bookViews>
@@ -557,18 +557,18 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" customWidth="1"/>
-    <col min="4" max="4" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -596,7 +596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -610,7 +610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -624,7 +624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -652,7 +652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -666,7 +666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -680,7 +680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -694,7 +694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -708,7 +708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -722,7 +722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -736,7 +736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -750,7 +750,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -764,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -778,7 +778,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -792,7 +792,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -806,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -820,7 +820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -834,7 +834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -848,7 +848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>

</xml_diff>